<commit_message>
Fixed 3 out of 11 broken existing tests
</commit_message>
<xml_diff>
--- a/demo_projects/simpel_vergelijkings_project/simpel_vergelijking_template4.xlsx
+++ b/demo_projects/simpel_vergelijkings_project/simpel_vergelijking_template4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\OTLMOW-GUI\demo_projects\simpel_vergelijkings_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF04DBE-925A-4FAF-8D7D-D6D8DE462021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CBA8D8-35B4-4CB6-ADFD-28E40DDD9D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ins#Verkeersbordopstelling" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="319">
   <si>
     <t>typeURI</t>
   </si>
@@ -268,18 +268,12 @@
     <t>dummy_zQp</t>
   </si>
   <si>
-    <t>dummy_Ej</t>
-  </si>
-  <si>
     <t>dummy_Q</t>
   </si>
   <si>
     <t>dummy_okopD</t>
   </si>
   <si>
-    <t>dummy_tCIvXsNGzb</t>
-  </si>
-  <si>
     <t>dummy_bcjseEAj</t>
   </si>
   <si>
@@ -292,18 +286,12 @@
     <t>dummy_a</t>
   </si>
   <si>
-    <t>dummy_PJfHLzi</t>
-  </si>
-  <si>
     <t>dummy_XKCZ</t>
   </si>
   <si>
     <t>dummy_zjqcP</t>
   </si>
   <si>
-    <t>dummy_sa</t>
-  </si>
-  <si>
     <t>dummy_v</t>
   </si>
   <si>
@@ -316,15 +304,9 @@
     <t>dummy_BMEYASLimy</t>
   </si>
   <si>
-    <t>dummy_G</t>
-  </si>
-  <si>
     <t>dummy_zmuNT</t>
   </si>
   <si>
-    <t>dummy_TOT</t>
-  </si>
-  <si>
     <t>dummy_nm</t>
   </si>
   <si>
@@ -511,15 +493,9 @@
     <t>dummy_LxexRM</t>
   </si>
   <si>
-    <t>dummy_qPvTVjcgQV</t>
-  </si>
-  <si>
     <t>dummy_Ouee</t>
   </si>
   <si>
-    <t>dummy_fvHaJ</t>
-  </si>
-  <si>
     <t>dummy_ZT</t>
   </si>
   <si>
@@ -529,18 +505,12 @@
     <t>dummy_WvbUTuNPl</t>
   </si>
   <si>
-    <t>dummy_qcUovGGd</t>
-  </si>
-  <si>
     <t>dummy_nwutvmJCp</t>
   </si>
   <si>
     <t>dummy_dygQREJZQr</t>
   </si>
   <si>
-    <t>dummy_lEUngoD</t>
-  </si>
-  <si>
     <t>dummy_Wk</t>
   </si>
   <si>
@@ -553,16 +523,10 @@
     <t>dummy_ecMhqot</t>
   </si>
   <si>
-    <t>dummy_OMnORzG</t>
-  </si>
-  <si>
     <t>dummy_zpYARLEyf</t>
   </si>
   <si>
     <t>dummy_nsG</t>
-  </si>
-  <si>
-    <t>dummy_tyg</t>
   </si>
   <si>
     <t>dummy_BwZwxE</t>
@@ -1361,7 +1325,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,11 +1625,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="1" width="64.7109375" customWidth="1"/>
+    <col min="2" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1711,22 +1678,22 @@
         <v>79</v>
       </c>
       <c r="D2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" t="s">
         <v>80</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>81</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" t="s">
         <v>82</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>83</v>
-      </c>
-      <c r="H2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" t="s">
-        <v>85</v>
       </c>
       <c r="J2" t="s">
         <v>30</v>
@@ -1737,28 +1704,28 @@
         <v>77</v>
       </c>
       <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" t="s">
         <v>86</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>87</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" t="s">
         <v>88</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>89</v>
-      </c>
-      <c r="F3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" t="s">
-        <v>93</v>
       </c>
       <c r="J3" t="s">
         <v>48</v>
@@ -1769,28 +1736,28 @@
         <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="E4" t="s">
         <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G4" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J4" t="s">
         <v>30</v>
@@ -1810,7 +1777,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1828,16 +1797,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1846,25 +1815,25 @@
         <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="N1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="O1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="P1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="Q1" t="s">
         <v>12</v>
@@ -1879,39 +1848,39 @@
         <v>17</v>
       </c>
       <c r="U1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" t="s">
         <v>112</v>
       </c>
-      <c r="B2" t="s">
+      <c r="I2" t="s">
         <v>113</v>
       </c>
-      <c r="C2" t="s">
+      <c r="J2" t="s">
         <v>114</v>
       </c>
-      <c r="D2" t="s">
+      <c r="K2" t="s">
         <v>115</v>
-      </c>
-      <c r="E2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" t="s">
-        <v>120</v>
-      </c>
-      <c r="K2" t="s">
-        <v>121</v>
       </c>
       <c r="L2" t="s">
         <v>30</v>
@@ -1923,54 +1892,54 @@
         <v>30</v>
       </c>
       <c r="O2" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>118</v>
+      </c>
+      <c r="R2" t="s">
+        <v>119</v>
+      </c>
+      <c r="S2" t="s">
+        <v>120</v>
+      </c>
+      <c r="T2" t="s">
+        <v>121</v>
+      </c>
+      <c r="U2" t="s">
         <v>122</v>
-      </c>
-      <c r="P2" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>124</v>
-      </c>
-      <c r="R2" t="s">
-        <v>125</v>
-      </c>
-      <c r="S2" t="s">
-        <v>126</v>
-      </c>
-      <c r="T2" t="s">
-        <v>127</v>
-      </c>
-      <c r="U2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" t="s">
+        <v>128</v>
+      </c>
+      <c r="J3" t="s">
         <v>129</v>
       </c>
-      <c r="C3" t="s">
+      <c r="K3" t="s">
         <v>130</v>
-      </c>
-      <c r="D3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H3" t="s">
-        <v>133</v>
-      </c>
-      <c r="I3" t="s">
-        <v>134</v>
-      </c>
-      <c r="J3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K3" t="s">
-        <v>136</v>
       </c>
       <c r="L3" t="s">
         <v>30</v>
@@ -1982,57 +1951,57 @@
         <v>30</v>
       </c>
       <c r="O3" t="s">
+        <v>131</v>
+      </c>
+      <c r="P3" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R3" t="s">
+        <v>134</v>
+      </c>
+      <c r="S3" t="s">
+        <v>135</v>
+      </c>
+      <c r="T3" t="s">
+        <v>136</v>
+      </c>
+      <c r="U3" t="s">
         <v>137</v>
-      </c>
-      <c r="P3" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>139</v>
-      </c>
-      <c r="R3" t="s">
-        <v>140</v>
-      </c>
-      <c r="S3" t="s">
-        <v>141</v>
-      </c>
-      <c r="T3" t="s">
-        <v>142</v>
-      </c>
-      <c r="U3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I4" t="s">
         <v>144</v>
       </c>
-      <c r="C4" t="s">
+      <c r="J4" t="s">
         <v>145</v>
       </c>
-      <c r="D4" t="s">
+      <c r="K4" t="s">
         <v>146</v>
-      </c>
-      <c r="E4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H4" t="s">
-        <v>149</v>
-      </c>
-      <c r="I4" t="s">
-        <v>150</v>
-      </c>
-      <c r="J4" t="s">
-        <v>151</v>
-      </c>
-      <c r="K4" t="s">
-        <v>152</v>
       </c>
       <c r="L4" t="s">
         <v>48</v>
@@ -2044,25 +2013,25 @@
         <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="P4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="Q4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="R4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="S4" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="T4" t="s">
         <v>36</v>
       </c>
       <c r="U4" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2098,7 +2067,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2140,31 +2109,31 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="E2" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G2" t="s">
-        <v>163</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
         <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="J2" t="s">
         <v>48</v>
@@ -2172,31 +2141,31 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" t="s">
         <v>159</v>
       </c>
-      <c r="B3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E3" t="s">
-        <v>168</v>
-      </c>
       <c r="F3" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="G3" t="s">
-        <v>170</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="I3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="J3" t="s">
         <v>30</v>
@@ -2204,31 +2173,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>175</v>
+        <v>212</v>
       </c>
       <c r="E4" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="F4" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="G4" t="s">
-        <v>178</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="I4" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="J4" t="s">
         <v>48</v>
@@ -2249,7 +2218,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,19 +2246,19 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="J1" t="s">
         <v>15</v>
       </c>
       <c r="K1" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="L1" t="s">
         <v>16</v>
@@ -2300,125 +2269,125 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D2" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="E2" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="H2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="I2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="J2" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="K2" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="L2" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="M2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" t="s">
         <v>184</v>
       </c>
-      <c r="B3" t="s">
-        <v>196</v>
-      </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="E3" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="F3" t="s">
         <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="H3" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="I3" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="J3" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="K3" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="L3" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="M3" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="E4" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="F4" t="s">
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="H4" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="I4" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="J4" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="K4" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="L4" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="M4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2453,7 +2422,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2474,31 +2445,31 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="H1" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="K1" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="L1" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="M1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="N1" t="s">
         <v>12</v>
@@ -2516,196 +2487,196 @@
         <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="T1" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="D2" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="E2" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F2" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="G2" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="H2" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="I2" t="s">
         <v>48</v>
       </c>
       <c r="J2" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="K2" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="L2" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="M2" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="N2" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="O2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="P2" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="Q2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="R2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="S2" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="T2" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="D3" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="E3" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="F3" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="G3" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="H3" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="I3" t="s">
         <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="K3" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="L3" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="M3" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="N3" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="O3" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="P3" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="Q3" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="R3" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="S3" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="T3" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="C4" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="D4" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="E4" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="F4" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="G4" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="H4" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="I4" t="s">
         <v>48</v>
       </c>
       <c r="J4" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="K4" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="L4" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="M4" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="N4" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="O4" t="s">
         <v>50</v>
       </c>
       <c r="P4" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="Q4" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="R4" t="s">
         <v>36</v>
       </c>
       <c r="S4" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="T4" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2755,71 +2726,71 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="B1" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="C1" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="D1" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="E1" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="F1" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="G1" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="B2" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="C2" t="s">
         <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="F2" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="G2" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="B3" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="F3" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="G3" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2830,39 +2801,39 @@
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="D4" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="E4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F4" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="G4" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="B5" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="D5" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E5" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="F5" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="G5" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2876,138 +2847,138 @@
         <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F6" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="G6" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="B7" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="D7" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="E7" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="F7" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="G7" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="D8" t="s">
         <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="F8" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="G8" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="D9" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E9" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="F9" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="E10" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="F10" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="E12" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="E13" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="E14" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="E15" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="E16" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -3017,22 +2988,22 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>